<commit_message>
Update performance dashboard 2026-01-06 19:02 - Simplified Design v3.1
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20260106.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20260106.xlsx
@@ -1524,26 +1524,26 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>¥1,000,296.80</t>
+          <t>¥1,000,689.80</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>¥+296.80</t>
+          <t>¥+689.80</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.07%</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>+0.63%</t>
+          <t>+1.35%</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-3.019</v>
+        <v>-1.201</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1552,24 +1552,24 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>54.5%</t>
+          <t>58.3%</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>0.0027%</t>
+          <t>0.0058%</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>0.4304%</t>
+          <t>0.4422%</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N15" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>20260105</t>
+          <t>20260106</t>
         </is>
       </c>
     </row>
@@ -2967,26 +2967,26 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>¥1,000,296.80</t>
+          <t>¥1,000,689.80</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>¥+296.80</t>
+          <t>¥+689.80</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>+0.03%</t>
+          <t>+0.07%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+0.63%</t>
+          <t>+1.35%</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>-3.019</v>
+        <v>-1.201</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2995,24 +2995,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>54.5%</t>
+          <t>58.3%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>0.0027%</t>
+          <t>0.0058%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>0.4304%</t>
+          <t>0.4422%</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N5" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>20260105</t>
+          <t>20260106</t>
         </is>
       </c>
     </row>

</xml_diff>